<commit_message>
sugestões relacionadas aos casos de uso
</commit_message>
<xml_diff>
--- a/Casos.de.Uso.xlsx
+++ b/Casos.de.Uso.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Educação\Christus\2016.1\APIS\Projeto Final\RogaMultiMarcas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>NUM</t>
   </si>
@@ -107,13 +112,34 @@
   </si>
   <si>
     <t>Confirmar a escolha do produto e forma de pagamento.</t>
+  </si>
+  <si>
+    <t>Do jeito que está me parece muito simplificado, parece que existem funcionalidades agregadas dentro de outras e/ou funcionalidades faltando, a saber:</t>
+  </si>
+  <si>
+    <t>Login - o texto menciona que o usuário pode alterar sua senha. Não vi esse caso de uso</t>
+  </si>
+  <si>
+    <t>Cadastro de Usuário - o usuário só pode se cadastrar? Não tem como alterar seus dados depois de cadastrado?</t>
+  </si>
+  <si>
+    <t>Visualizar itens (um conjunto de itens, normalmente em uma lista), é diferente de visualizar um produto. Necessita ser melhorada essa questão. Normalmente é feita uma consulta, por nome ou categoria, e exibida uma lista de produtos que atendem a pesquisa. Deveria haver uma funcionalidade para isso.</t>
+  </si>
+  <si>
+    <t>Selecionar Produto é uma coisa e adicionar ao carrinho é outra. Não vi nada para adicionar ao carrinho. Também não vi nada para remover do carrinho</t>
+  </si>
+  <si>
+    <t>Comprar também é uma funcionalidade muito genérica. E também tem que ter o pagamento como uma funcionalidade separada.</t>
+  </si>
+  <si>
+    <t>Deveria existir também um caso de uso para manter as categorias dos produtos do site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -122,6 +148,17 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -144,15 +181,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -199,7 +249,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,9 +281,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -265,6 +316,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -440,11 +492,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -454,7 +506,7 @@
     <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -488,7 +540,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -505,7 +557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -522,7 +574,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -539,7 +591,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -556,7 +608,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -573,33 +625,70 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B12" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="39.75" customHeight="1">
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B14" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+      <c r="B16" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B13:F13"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>